<commit_message>
REFACTORING: rename types to categories, add HOCs
</commit_message>
<xml_diff>
--- a/backend/backend-app/src/main/resources/xlsx/user-template.xlsx
+++ b/backend/backend-app/src/main/resources/xlsx/user-template.xlsx
@@ -50,16 +50,16 @@
     <t>Results of the year</t>
   </si>
   <si>
-    <t>inc. type 1</t>
+    <t>inc. category 2</t>
   </si>
   <si>
-    <t>inc. type 2</t>
+    <t>inc. category 1</t>
   </si>
   <si>
-    <t>exp. type 1</t>
+    <t>exp. category 1</t>
   </si>
   <si>
-    <t>exp. type 2</t>
+    <t>exp. category 2</t>
   </si>
 </sst>
 </file>
@@ -571,7 +571,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -609,10 +609,10 @@
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="19"/>
       <c r="B2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>9</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>0</v>
@@ -1383,7 +1383,7 @@
         <v>44562</v>
       </c>
       <c r="B35" s="9">
-        <f t="shared" ref="B35:G35" si="3">SUMPRODUCT(B4:B34,--(MONTH($A4:$A34)=MONTH($A35)))</f>
+        <f t="shared" ref="B35:F35" si="3">SUMPRODUCT(B4:B34,--(MONTH($A4:$A34)=MONTH($A35)))</f>
         <v>10</v>
       </c>
       <c r="C35" s="9">
@@ -2059,7 +2059,7 @@
         <v>44593</v>
       </c>
       <c r="B64" s="9">
-        <f t="shared" ref="B64:G64" si="5">SUMPRODUCT(B33:B63,--(MONTH($A33:$A63)=MONTH($A64)))</f>
+        <f t="shared" ref="B64:F64" si="5">SUMPRODUCT(B33:B63,--(MONTH($A33:$A63)=MONTH($A64)))</f>
         <v>0</v>
       </c>
       <c r="C64" s="9">
@@ -2804,7 +2804,7 @@
         <v>44621</v>
       </c>
       <c r="B96" s="9">
-        <f t="shared" ref="B96:G96" si="9">SUMPRODUCT(B65:B95,--(MONTH($A65:$A95)=MONTH($A96)))</f>
+        <f t="shared" ref="B96:F96" si="9">SUMPRODUCT(B65:B95,--(MONTH($A65:$A95)=MONTH($A96)))</f>
         <v>0</v>
       </c>
       <c r="C96" s="9">
@@ -3526,7 +3526,7 @@
         <v>44652</v>
       </c>
       <c r="B127" s="9">
-        <f t="shared" ref="B127:G127" si="11">SUMPRODUCT(B96:B126,--(MONTH($A96:$A126)=MONTH($A127)))</f>
+        <f t="shared" ref="B127:F127" si="11">SUMPRODUCT(B96:B126,--(MONTH($A96:$A126)=MONTH($A127)))</f>
         <v>0</v>
       </c>
       <c r="C127" s="9">
@@ -4271,7 +4271,7 @@
         <v>44682</v>
       </c>
       <c r="B159" s="9">
-        <f t="shared" ref="B159:G159" si="15">SUMPRODUCT(B128:B158,--(MONTH($A128:$A158)=MONTH($A159)))</f>
+        <f t="shared" ref="B159:F159" si="15">SUMPRODUCT(B128:B158,--(MONTH($A128:$A158)=MONTH($A159)))</f>
         <v>0</v>
       </c>
       <c r="C159" s="9">
@@ -4993,7 +4993,7 @@
         <v>44713</v>
       </c>
       <c r="B190" s="9">
-        <f t="shared" ref="B190:G190" si="17">SUMPRODUCT(B159:B189,--(MONTH($A159:$A189)=MONTH($A190)))</f>
+        <f t="shared" ref="B190:F190" si="17">SUMPRODUCT(B159:B189,--(MONTH($A159:$A189)=MONTH($A190)))</f>
         <v>0</v>
       </c>
       <c r="C190" s="9">
@@ -5738,7 +5738,7 @@
         <v>44743</v>
       </c>
       <c r="B222" s="9">
-        <f t="shared" ref="B222:G222" si="21">SUMPRODUCT(B191:B221,--(MONTH($A191:$A221)=MONTH($A222)))</f>
+        <f t="shared" ref="B222:F222" si="21">SUMPRODUCT(B191:B221,--(MONTH($A191:$A221)=MONTH($A222)))</f>
         <v>0</v>
       </c>
       <c r="C222" s="9">
@@ -6483,7 +6483,7 @@
         <v>44774</v>
       </c>
       <c r="B254" s="9">
-        <f t="shared" ref="B254:G254" si="23">SUMPRODUCT(B223:B253,--(MONTH($A223:$A253)=MONTH($A254)))</f>
+        <f t="shared" ref="B254:F254" si="23">SUMPRODUCT(B223:B253,--(MONTH($A223:$A253)=MONTH($A254)))</f>
         <v>0</v>
       </c>
       <c r="C254" s="9">
@@ -7205,7 +7205,7 @@
         <v>44805</v>
       </c>
       <c r="B285" s="9">
-        <f t="shared" ref="B285:G285" si="27">SUMPRODUCT(B254:B284,--(MONTH($A254:$A284)=MONTH($A285)))</f>
+        <f t="shared" ref="B285:F285" si="27">SUMPRODUCT(B254:B284,--(MONTH($A254:$A284)=MONTH($A285)))</f>
         <v>0</v>
       </c>
       <c r="C285" s="9">
@@ -7950,7 +7950,7 @@
         <v>44835</v>
       </c>
       <c r="B317" s="9">
-        <f t="shared" ref="B317:G317" si="29">SUMPRODUCT(B286:B316,--(MONTH($A286:$A316)=MONTH($A317)))</f>
+        <f t="shared" ref="B317:F317" si="29">SUMPRODUCT(B286:B316,--(MONTH($A286:$A316)=MONTH($A317)))</f>
         <v>0</v>
       </c>
       <c r="C317" s="9">
@@ -8672,7 +8672,7 @@
         <v>44866</v>
       </c>
       <c r="B348" s="9">
-        <f t="shared" ref="B348:G348" si="33">SUMPRODUCT(B317:B347,--(MONTH($A317:$A347)=MONTH($A348)))</f>
+        <f t="shared" ref="B348:F348" si="33">SUMPRODUCT(B317:B347,--(MONTH($A317:$A347)=MONTH($A348)))</f>
         <v>0</v>
       </c>
       <c r="C348" s="9">
@@ -9417,7 +9417,7 @@
         <v>44896</v>
       </c>
       <c r="B380" s="9">
-        <f t="shared" ref="B380:G380" si="35">SUMPRODUCT(B349:B379,--(MONTH($A349:$A379)=MONTH($A380)))</f>
+        <f t="shared" ref="B380:F380" si="35">SUMPRODUCT(B349:B379,--(MONTH($A349:$A379)=MONTH($A380)))</f>
         <v>0</v>
       </c>
       <c r="C380" s="9">

</xml_diff>